<commit_message>
pulp factory complete and tested
</commit_message>
<xml_diff>
--- a/data/paper/factories/pulp_factory-0C.xlsx
+++ b/data/paper/factories/pulp_factory-0C.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\BlackBlox\data\paper\factories\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/paper/factories/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC3E449-E1B2-8F44-9F92-8F09379772A6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="465" windowWidth="17055" windowHeight="17535" activeTab="1"/>
+    <workbookView xWindow="1200" yWindow="460" windowWidth="19740" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="chains" sheetId="9" r:id="rId1"/>
@@ -22,18 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="52">
   <si>
     <t>Inflow</t>
   </si>
@@ -131,18 +126,12 @@
     <t>liquor</t>
   </si>
   <si>
-    <t>white liquor</t>
-  </si>
-  <si>
     <t>weak black liquor</t>
   </si>
   <si>
     <t>paper_chipping</t>
   </si>
   <si>
-    <t>paper_pulpling</t>
-  </si>
-  <si>
     <t>paper_bleaching</t>
   </si>
   <si>
@@ -174,13 +163,34 @@
   </si>
   <si>
     <t>simple_WWT</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>power</t>
+  </si>
+  <si>
+    <t>electricity</t>
+  </si>
+  <si>
+    <t>simple_power</t>
+  </si>
+  <si>
+    <t>CONSUMED white liquor</t>
+  </si>
+  <si>
+    <t>paper_pulping</t>
+  </si>
+  <si>
+    <t>wet hog fuel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -215,6 +225,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -237,7 +254,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -246,10 +263,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -560,21 +578,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
-    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -591,7 +609,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -605,12 +623,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -620,9 +638,9 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>28</v>
@@ -631,10 +649,10 @@
         <v>4</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -648,21 +666,21 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -676,13 +694,24 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E10" s="1"/>
     </row>
   </sheetData>
@@ -691,29 +720,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.875" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" customWidth="1"/>
     <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -748,127 +777,349 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>31</v>
       </c>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="3"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B13" s="3"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B14" s="3"/>
       <c r="E14" s="5"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E15" s="5"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E16" s="5"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="E17" s="5"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="E18" s="5"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" s="1"/>
       <c r="D19" s="2"/>
       <c r="E19" s="5"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="E21" s="5"/>
       <c r="G21" s="1"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="E22" s="5"/>
       <c r="G22" s="1"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="E23" s="5"/>
       <c r="G23" s="1"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="E24" s="5"/>
       <c r="G24" s="1"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
       <c r="G25" s="1"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
       <c r="G26" s="1"/>
       <c r="H26" s="5"/>
     </row>
@@ -878,21 +1129,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="2"/>
-    <col min="2" max="2" width="18.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.875" style="2"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -903,45 +1154,45 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="C4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
     </row>
@@ -951,20 +1202,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -975,26 +1226,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>